<commit_message>
updating files: dim_bancos and dim_contas
</commit_message>
<xml_diff>
--- a/dataset/PlanoContas.xlsx
+++ b/dataset/PlanoContas.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\_rma\_tecnologia\_data\evolve_data\projetos\projeto_fluxo_de_caixa_evolve\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8734D148-B211-4836-A73C-ACC1961DF281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95AE87-C52F-4AEF-8000-FA7D77C4AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{752E5475-DC94-4FA9-B84E-2B77A75F99A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{752E5475-DC94-4FA9-B84E-2B77A75F99A9}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanoContas" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>Receitas com vendas</t>
   </si>
@@ -210,6 +211,9 @@
   </si>
   <si>
     <t>Nome da conta contábil, detalhando o item específico de receita, despesa, imposto ou investimento.</t>
+  </si>
+  <si>
+    <t>Tabela: dim_contas</t>
   </si>
 </sst>
 </file>
@@ -655,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4D7506-AC81-431C-A149-2785727B75D7}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1143,4 +1147,83 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98ABF050-0C2F-4CD5-8580-BC4168A8F0BB}">
+  <dimension ref="B2:D8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="39.950000000000003" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="39.950000000000003" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="39.950000000000003" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="39.950000000000003" customHeight="1">
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>